<commit_message>
Update job listings - 2025-11-07 11:59:14
</commit_message>
<xml_diff>
--- a/jobs.xlsx
+++ b/jobs.xlsx
@@ -1,75 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Jobs" sheetId="1" r:id="rId1"/>
+    <sheet name="Jobs" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Source</t>
-  </si>
-  <si>
-    <t>Date_Found</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Salary</t>
-  </si>
-  <si>
-    <t>Experience</t>
-  </si>
-  <si>
-    <t>Posted</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -84,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -400,46 +420,548 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="31" customWidth="1" min="2" max="2"/>
+    <col width="29" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="12" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Company</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Location</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Link</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Source</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Date_Found</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Posted</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Salary</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Data Science Intern</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Arctan</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Bengaluru, Karnataka, India</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>https://in.linkedin.com/jobs/view/data-science-intern-at-arctan-4321242862?position=1&amp;pageNum=0&amp;refId=%2Fa%2FK5%2FbehX1X3ORENgvnXQ%3D%3D&amp;trackingId=dmLdUG%2FRhcMfzBEGBJdsSQ%3D%3D</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2025-11-06</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AI Engineer, Intern</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Newfold Digital</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Mumbai Metropolitan Region</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>https://in.linkedin.com/jobs/view/ai-engineer-intern-at-newfold-digital-4300861727?position=2&amp;pageNum=0&amp;refId=%2Fa%2FK5%2FbehX1X3ORENgvnXQ%3D%3D&amp;trackingId=9e5RZbd1Ql08Yzb4VcUDpg%3D%3D</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2025-11-06</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Data Science Internship in Mumbai</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Faclon Labs</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Mumbai Metropolitan Region</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>https://in.linkedin.com/jobs/view/data-science-internship-in-mumbai-at-faclon-labs-4334840753?position=3&amp;pageNum=0&amp;refId=%2Fa%2FK5%2FbehX1X3ORENgvnXQ%3D%3D&amp;trackingId=ivWEX3bu%2B76hPHf4wWz2xQ%3D%3D</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Python Developer Intern</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Webs IT Solution</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>https://in.linkedin.com/jobs/view/python-developer-intern-at-webs-it-solution-4334733482?position=4&amp;pageNum=0&amp;refId=%2Fa%2FK5%2FbehX1X3ORENgvnXQ%3D%3D&amp;trackingId=S19%2BJQCxvA%2FRaYKU2qHb%2BQ%3D%3D</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Data Science Intern</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>WEBBOOST SOLUTION IT SERVICES</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>https://in.linkedin.com/jobs/view/data-science-intern-at-webboost-solution-it-services-4334833119?position=5&amp;pageNum=0&amp;refId=%2Fa%2FK5%2FbehX1X3ORENgvnXQ%3D%3D&amp;trackingId=ylGlmBQhiwVcJhHaiocQ1Q%3D%3D</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Python Developer Intern</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>WEBBOOST SOLUTION IT SERVICES</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>https://in.linkedin.com/jobs/view/python-developer-intern-at-webboost-solution-it-services-4334753531?position=6&amp;pageNum=0&amp;refId=%2Fa%2FK5%2FbehX1X3ORENgvnXQ%3D%3D&amp;trackingId=t7IfMojkLbWbCo7h15Uwxw%3D%3D</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Data Science Intern</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>UM IT Solutions</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>https://in.linkedin.com/jobs/view/data-science-intern-at-um-it-solutions-4321066791?position=7&amp;pageNum=0&amp;refId=%2Fa%2FK5%2FbehX1X3ORENgvnXQ%3D%3D&amp;trackingId=pEulRWmmyASl%2FD43kjfBXQ%3D%3D</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Intern – AI Engineer</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Kaleris</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Chennai, Tamil Nadu, India</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>https://in.linkedin.com/jobs/view/intern-%E2%80%93-ai-engineer-at-kaleris-4295837872?position=8&amp;pageNum=0&amp;refId=%2Fa%2FK5%2FbehX1X3ORENgvnXQ%3D%3D&amp;trackingId=Wm0qmHUfaLXRZ5ETTi93Gg%3D%3D</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>2025-11-06</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence Intern</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>WEBBOOST SOLUTION IT SERVICES</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>India</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>https://in.linkedin.com/jobs/view/artificial-intelligence-intern-at-webboost-solution-it-services-4334665587?position=1&amp;pageNum=0&amp;refId=b698TkhLUv5nig10JQIeDA%3D%3D&amp;trackingId=%2FC6Wg2%2FTvpKyO3wZlDlDOw%3D%3D</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Flutter Engineer (Fresher)</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Unlimits</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Noida, Uttar Pradesh, India</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>https://in.linkedin.com/jobs/view/flutter-engineer-fresher-at-unlimits-4338111877?position=1&amp;pageNum=0&amp;refId=cKACyrJHmGuFlnKhzEr0%2BA%3D%3D&amp;trackingId=Ab968oUNZ2Szq8BLiLxFNg%3D%3D</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>LinkedIn</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>2025-11-07</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Not disclosed</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>